<commit_message>
Updated pathway comparison counting sheet
</commit_message>
<xml_diff>
--- a/Data/pathway_comparison.xlsx
+++ b/Data/pathway_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snorres\git\BiGMeC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3B1F62-99B2-4B4B-9373-BA046C71D0B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551DF9C6-CF20-444D-AA36-421F85A70E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="3045" windowWidth="14400" windowHeight="8415" xr2:uid="{27EB3488-87F4-42D4-896F-D101A3B5911A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{27EB3488-87F4-42D4-896F-D101A3B5911A}"/>
   </bookViews>
   <sheets>
     <sheet name="bafilomycin" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="225">
   <si>
     <t>Domain number</t>
   </si>
@@ -660,9 +660,6 @@
     <t>3-Phospho-D-glyceroyl phosphate + H+ + NADPH -&gt; NADP+ + Phosphate</t>
   </si>
   <si>
-    <t>formic acid + glycine-&gt; H2O + N-formyl glycine</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -&gt; H2O (cyclisation)</t>
   </si>
   <si>
@@ -707,9 +704,6 @@
     </r>
   </si>
   <si>
-    <t>leu5, leu6 and leu9</t>
-  </si>
-  <si>
     <t>X/C/PCP</t>
   </si>
   <si>
@@ -960,9 +954,6 @@
     <t>3-Hydroxyoctanoyl-CoA -&gt; CoA</t>
   </si>
   <si>
-    <t>L-Proline + ATP -&gt; AMP + H2O + Diphosphate</t>
-  </si>
-  <si>
     <t>2,3-didehydrobutyrine is modified from threonine by PTM (Ongey and Neubauer, 2016)</t>
   </si>
   <si>
@@ -1005,6 +996,15 @@
   </si>
   <si>
     <t>aptA1 and aptA2 are alternatives for the load and first extending module</t>
+  </si>
+  <si>
+    <t>formic acid + Glycine-&gt; H2O + N-formyl glycine</t>
+  </si>
+  <si>
+    <t>leu5, leu6, leu7 and leu9</t>
+  </si>
+  <si>
+    <t>L-Proline + ATP + FAD -&gt; AMP + H2O + Diphosphate + FADH2</t>
   </si>
 </sst>
 </file>
@@ -1401,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41C1A4B-DB7A-40AB-883A-B2D43A0727CE}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1575,10 +1575,10 @@
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -2896,7 +2896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F85781D-1E25-4764-A357-8FB194A18198}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -3060,10 +3060,10 @@
         <v>6</v>
       </c>
       <c r="G16" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="H16" t="s">
         <v>192</v>
-      </c>
-      <c r="H16" t="s">
-        <v>194</v>
       </c>
       <c r="I16">
         <f>(G16=H16)*1</f>
@@ -4818,7 +4818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5961845-BCBB-45A8-A342-C900AC1949AA}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -6449,7 +6449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CE930B-A3F9-40DC-8298-316EA032E6AF}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -6502,12 +6502,12 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -6592,7 +6592,7 @@
         <v>24</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>25</v>
@@ -6621,10 +6621,10 @@
         <v>104</v>
       </c>
       <c r="G16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -7668,8 +7668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EFC036-77D9-48D1-A7E4-43D43CEA5AF4}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="E6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7818,7 +7818,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>25</v>
@@ -7844,7 +7844,7 @@
         <v>110</v>
       </c>
       <c r="H16" t="s">
-        <v>140</v>
+        <v>222</v>
       </c>
       <c r="J16">
         <f>(H16=I16)*1</f>
@@ -9251,7 +9251,7 @@
         <v>137</v>
       </c>
       <c r="G52" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
@@ -9452,7 +9452,7 @@
         <v>100</v>
       </c>
       <c r="H57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
@@ -9476,13 +9476,13 @@
         <v>43</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C58" s="4">
         <v>16</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I58" t="s">
         <v>139</v>
@@ -9532,8 +9532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA1C1EA-F874-45F1-B125-27437C296F50}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9554,7 +9554,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -9562,7 +9562,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9572,7 +9572,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -9580,7 +9580,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -9588,7 +9588,7 @@
         <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -9673,7 +9673,7 @@
         <v>24</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>25</v>
@@ -9687,25 +9687,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>148</v>
+        <v>223</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="H16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I16">
         <f>(G16=H16)*1</f>
@@ -9728,22 +9728,22 @@
         <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F17" t="s">
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I17">
         <f t="shared" ref="I17:I34" si="0">(G17=H17)*1</f>
@@ -9766,25 +9766,25 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
@@ -9808,7 +9808,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C19" s="4">
         <v>2</v>
@@ -9823,7 +9823,7 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H19" t="s">
         <v>13</v>
@@ -9850,7 +9850,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C20" s="4">
         <v>2</v>
@@ -9892,7 +9892,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C21" s="4">
         <v>2</v>
@@ -9934,7 +9934,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C22" s="4">
         <v>3</v>
@@ -9976,7 +9976,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C23" s="4">
         <v>3</v>
@@ -10018,7 +10018,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C24" s="4">
         <v>3</v>
@@ -10060,7 +10060,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C25" s="4">
         <v>3</v>
@@ -10099,7 +10099,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C26" s="4">
         <v>4</v>
@@ -10141,7 +10141,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C27" s="4">
         <v>4</v>
@@ -10183,7 +10183,7 @@
         <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C28" s="4">
         <v>4</v>
@@ -10225,7 +10225,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C29" s="4">
         <v>5</v>
@@ -10267,7 +10267,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C30" s="4">
         <v>5</v>
@@ -10309,7 +10309,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C31" s="4">
         <v>5</v>
@@ -10351,7 +10351,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C32" s="4">
         <v>5</v>
@@ -10390,7 +10390,7 @@
         <v>18</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C33" s="4">
         <v>6</v>
@@ -10405,10 +10405,10 @@
         <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
@@ -10432,7 +10432,7 @@
         <v>19</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C34" s="4">
         <v>6</v>
@@ -10590,7 +10590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC06FBB-A8B3-48B1-B34B-75F42D9062B2}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" workbookViewId="0">
+    <sheetView topLeftCell="G15" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -10613,7 +10613,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -10621,7 +10621,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -10631,7 +10631,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -10639,7 +10639,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -10647,7 +10647,7 @@
         <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -10735,7 +10735,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>25</v>
@@ -10752,22 +10752,22 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E16" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F16" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G16" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J16">
         <f>(H16=I16)*1</f>
@@ -10790,13 +10790,13 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
         <v>100</v>
@@ -10805,13 +10805,13 @@
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -10833,13 +10833,13 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C18" s="4">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E18" t="s">
         <v>100</v>
@@ -10848,10 +10848,10 @@
         <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -10873,13 +10873,13 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C19" s="4">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E19" t="s">
         <v>100</v>
@@ -10888,7 +10888,7 @@
         <v>100</v>
       </c>
       <c r="H19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I19" t="s">
         <v>135</v>
@@ -10913,13 +10913,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C20" s="4">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E20" t="s">
         <v>100</v>
@@ -10928,10 +10928,10 @@
         <v>100</v>
       </c>
       <c r="H20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -10953,13 +10953,13 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C21" s="4">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
         <v>100</v>
@@ -10968,10 +10968,10 @@
         <v>100</v>
       </c>
       <c r="H21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -10993,13 +10993,13 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C22" s="4">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E22" t="s">
         <v>100</v>
@@ -11008,7 +11008,7 @@
         <v>100</v>
       </c>
       <c r="H22" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I22" t="s">
         <v>135</v>
@@ -11033,13 +11033,13 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C23" s="4">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E23" t="s">
         <v>100</v>
@@ -11048,10 +11048,10 @@
         <v>100</v>
       </c>
       <c r="H23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -11073,13 +11073,13 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C24" s="4">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
         <v>100</v>
@@ -11088,10 +11088,10 @@
         <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -11113,13 +11113,13 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C25" s="4">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E25" t="s">
         <v>100</v>
@@ -11128,10 +11128,10 @@
         <v>100</v>
       </c>
       <c r="H25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -11153,13 +11153,13 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C26" s="4">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E26" t="s">
         <v>100</v>
@@ -11168,10 +11168,10 @@
         <v>100</v>
       </c>
       <c r="H26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -11193,13 +11193,13 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C27" s="4">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E27" t="s">
         <v>100</v>
@@ -11208,10 +11208,10 @@
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -11233,13 +11233,13 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C28" s="4">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E28" t="s">
         <v>100</v>
@@ -11248,10 +11248,10 @@
         <v>100</v>
       </c>
       <c r="H28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -11273,13 +11273,13 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C29" s="4">
         <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E29" t="s">
         <v>100</v>
@@ -11288,10 +11288,10 @@
         <v>100</v>
       </c>
       <c r="H29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -11313,13 +11313,13 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C30" s="4">
         <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E30" t="s">
         <v>100</v>
@@ -11328,10 +11328,10 @@
         <v>100</v>
       </c>
       <c r="H30" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -11353,13 +11353,13 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C31" s="4">
         <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E31" t="s">
         <v>100</v>
@@ -11368,10 +11368,10 @@
         <v>100</v>
       </c>
       <c r="H31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -11393,13 +11393,13 @@
         <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C32" s="4">
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E32" t="s">
         <v>100</v>
@@ -11408,10 +11408,10 @@
         <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -11433,13 +11433,13 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C33" s="4">
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E33" t="s">
         <v>100</v>
@@ -11448,10 +11448,10 @@
         <v>100</v>
       </c>
       <c r="H33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I33" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -11473,13 +11473,13 @@
         <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C34" s="4">
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E34" t="s">
         <v>100</v>
@@ -11488,10 +11488,10 @@
         <v>100</v>
       </c>
       <c r="H34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I34" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -11513,7 +11513,7 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C35" s="4">
         <v>18</v>
@@ -11631,7 +11631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B956210-96A1-4A20-8605-6CC9FD28F634}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -11654,7 +11654,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -11662,7 +11662,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -11672,7 +11672,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -11680,7 +11680,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -11688,7 +11688,7 @@
         <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -11776,7 +11776,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>25</v>
@@ -11790,25 +11790,25 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F16" t="s">
         <v>138</v>
       </c>
       <c r="G16" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J16">
         <f>(H16=I16)*1</f>
@@ -11831,22 +11831,22 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F17" t="s">
         <v>100</v>
       </c>
       <c r="I17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J17">
         <f t="shared" ref="J17:J25" si="0">(H17=I17)*1</f>
@@ -11869,25 +11869,25 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F18" t="s">
         <v>138</v>
       </c>
       <c r="H18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
@@ -11910,25 +11910,25 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F19" t="s">
         <v>100</v>
       </c>
       <c r="H19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
@@ -11951,7 +11951,7 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C20" s="4">
         <v>2</v>
@@ -11966,10 +11966,10 @@
         <v>100</v>
       </c>
       <c r="H20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
@@ -11992,7 +11992,7 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C21" s="4">
         <v>3</v>
@@ -12007,10 +12007,10 @@
         <v>100</v>
       </c>
       <c r="H21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
@@ -12033,7 +12033,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C22" s="4">
         <v>4</v>
@@ -12048,10 +12048,10 @@
         <v>100</v>
       </c>
       <c r="H22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
@@ -12112,7 +12112,7 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C24" s="4">
         <v>5</v>
@@ -12127,10 +12127,10 @@
         <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>

</xml_diff>